<commit_message>
Doc updates and joystick axis remapping
</commit_message>
<xml_diff>
--- a/docs/FRC Status Lights.xlsx
+++ b/docs/FRC Status Lights.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaudets\Documents\repos\2017repo\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27792" windowHeight="12588"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="94">
   <si>
     <t>RoboRio</t>
   </si>
@@ -207,8 +212,89 @@
     <t>Long Blink</t>
   </si>
   <si>
+    <t>Talon-SRX Motor Controller</t>
+  </si>
+  <si>
+    <t>"Stat"</t>
+  </si>
+  <si>
+    <t>"Comm"</t>
+  </si>
+  <si>
+    <t>2 Status LEDs</t>
+  </si>
+  <si>
+    <t>Alternate</t>
+  </si>
+  <si>
+    <t>State 1</t>
+  </si>
+  <si>
+    <t>State 2</t>
+  </si>
+  <si>
+    <t>Slow Red</t>
+  </si>
+  <si>
+    <t>Fast Red</t>
+  </si>
+  <si>
+    <t>Both on</t>
+  </si>
+  <si>
+    <t>Forward throttle (proportional to duty cycle)</t>
+  </si>
+  <si>
+    <t>Reverse throttle (proportional to duty cycle)</t>
+  </si>
+  <si>
+    <t>No power</t>
+  </si>
+  <si>
+    <t>CAN bus detected, robot disabled</t>
+  </si>
+  <si>
+    <t>Can bus/PWM is not detected</t>
+  </si>
+  <si>
+    <t>Fault detected</t>
+  </si>
+  <si>
+    <t>Forward limit switch or soft limit</t>
+  </si>
+  <si>
+    <t>Reverse limit switch or soft limit</t>
+  </si>
+  <si>
+    <t>Strobe M+</t>
+  </si>
+  <si>
+    <t>Strobe M-</t>
+  </si>
+  <si>
+    <t>Calibration mode</t>
+  </si>
+  <si>
+    <t>Successful calibration</t>
+  </si>
+  <si>
+    <t>Failed calibration</t>
+  </si>
+  <si>
+    <t>B/C CAL LED</t>
+  </si>
+  <si>
+    <t>Brake mode</t>
+  </si>
+  <si>
+    <t>Coast mode</t>
+  </si>
+  <si>
+    <t>M+ Altern.</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">No CAN comms or Solenoid fault            (blinks </t>
+      <t xml:space="preserve">No CAN comms or Solenoid fault                        (blinks </t>
     </r>
     <r>
       <rPr>
@@ -231,85 +317,13 @@
     </r>
   </si>
   <si>
-    <t>Talon-SRX Motor Controller</t>
-  </si>
-  <si>
-    <t>"Stat"</t>
-  </si>
-  <si>
-    <t>"Comm"</t>
-  </si>
-  <si>
-    <t>2 Status LEDs</t>
-  </si>
-  <si>
-    <t>Alternate</t>
-  </si>
-  <si>
-    <t>State 1</t>
-  </si>
-  <si>
-    <t>State 2</t>
-  </si>
-  <si>
-    <t>Slow Red</t>
-  </si>
-  <si>
-    <t>Fast Red</t>
-  </si>
-  <si>
-    <t>Both on</t>
-  </si>
-  <si>
-    <t>Forward throttle (proportional to duty cycle)</t>
-  </si>
-  <si>
-    <t>Reverse throttle (proportional to duty cycle)</t>
-  </si>
-  <si>
-    <t>No power</t>
-  </si>
-  <si>
-    <t>CAN bus detected, robot disabled</t>
-  </si>
-  <si>
-    <t>Can bus/PWM is not detected</t>
-  </si>
-  <si>
-    <t>Fault detected</t>
-  </si>
-  <si>
-    <t>Forward limit switch or soft limit</t>
-  </si>
-  <si>
-    <t>Reverse limit switch or soft limit</t>
-  </si>
-  <si>
-    <t>Strobe M+</t>
-  </si>
-  <si>
-    <t>Strobe M-</t>
-  </si>
-  <si>
-    <t>Calibration mode</t>
-  </si>
-  <si>
-    <t>Successful calibration</t>
-  </si>
-  <si>
-    <t>Failed calibration</t>
-  </si>
-  <si>
-    <t>B/C CAL LED</t>
-  </si>
-  <si>
-    <t>Brake mode</t>
-  </si>
-  <si>
-    <t>Coast mode</t>
-  </si>
-  <si>
-    <t>M+ Altern.</t>
+    <t>*</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>* = normal operation state</t>
   </si>
 </sst>
 </file>
@@ -577,9 +591,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -639,12 +650,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -660,11 +665,2160 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="262">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1150,6 +3304,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1443,7 +3600,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1478,7 +3635,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1690,391 +3847,416 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G77"/>
+  <dimension ref="B1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="2.42578125" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="9"/>
-    <col min="6" max="6" width="38.7109375" style="26" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="2.44140625" customWidth="1"/>
+    <col min="3" max="5" width="9.109375" style="9"/>
+    <col min="6" max="6" width="38.6640625" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" ht="21" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
-      <c r="F1" s="20"/>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="20"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="20"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="16" t="s">
+      <c r="F3" s="19"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="27"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F4" s="26"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="18"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="40" t="s">
+        <v>91</v>
+      </c>
       <c r="C6" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="28"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F6" s="27"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C7" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="28"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="27"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C8" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="28"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F8" s="27"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="23"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="13"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C10" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="28"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F10" s="27"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="40" t="s">
+        <v>91</v>
+      </c>
       <c r="C11" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="28"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F11" s="27"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C12" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="28"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F12" s="27"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C13" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="28"/>
-    </row>
-    <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="27"/>
+    </row>
+    <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="34"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F14" s="39"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C15" s="11" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="28"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F15" s="27"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="12" t="s">
+      <c r="C16" s="13"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="29"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F17" s="28"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="18"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C19" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="28"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F19" s="27"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C20" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="32" t="s">
+      <c r="E20" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="28"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F20" s="27"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C21" s="11" t="s">
         <v>34</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="32" t="s">
+      <c r="E21" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="28"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="27"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="40" t="s">
+        <v>91</v>
+      </c>
       <c r="C22" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="32" t="s">
+      <c r="E22" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="28"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F22" s="27"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="18"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="13" t="s">
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="17"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C24" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="28"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F24" s="27"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C25" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="32" t="s">
+      <c r="E25" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="28"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="27"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="40" t="s">
+        <v>91</v>
+      </c>
       <c r="C26" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E26" s="32" t="s">
+      <c r="E26" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="F26" s="28"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F26" s="27"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C27" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="32" t="s">
+      <c r="E27" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F27" s="28"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="27"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="18"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="13"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C29" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E29" s="30" t="s">
+      <c r="E29" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="23"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="40" t="s">
+        <v>91</v>
+      </c>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="30" t="s">
+      <c r="E30" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="F30" s="23"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F30" s="22"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C31" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="F31" s="23"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F31" s="22"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C32" s="2"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="25"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="24"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="25"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="16" t="s">
+      <c r="F33" s="24"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C34" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D34" s="17" t="s">
+      <c r="D34" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F34" s="21" t="s">
+      <c r="F34" s="20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35" s="40" t="s">
+        <v>91</v>
+      </c>
       <c r="C35" s="11" t="s">
         <v>34</v>
       </c>
@@ -2084,11 +4266,11 @@
       <c r="E35" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F35" s="24" t="s">
+      <c r="F35" s="23" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C36" s="11" t="s">
         <v>34</v>
       </c>
@@ -2098,11 +4280,11 @@
       <c r="E36" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F36" s="24" t="s">
+      <c r="F36" s="23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C37" s="11" t="s">
         <v>34</v>
       </c>
@@ -2112,11 +4294,11 @@
       <c r="E37" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F37" s="24" t="s">
+      <c r="F37" s="23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C38" s="11" t="s">
         <v>28</v>
       </c>
@@ -2126,11 +4308,11 @@
       <c r="E38" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F38" s="24" t="s">
+      <c r="F38" s="23" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C39" s="11" t="s">
         <v>28</v>
       </c>
@@ -2140,11 +4322,11 @@
       <c r="E39" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F39" s="24" t="s">
+      <c r="F39" s="23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C40" s="11" t="s">
         <v>20</v>
       </c>
@@ -2154,99 +4336,104 @@
       <c r="E40" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F40" s="24" t="s">
+      <c r="F40" s="23" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C41" s="2"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
-      <c r="F41" s="25"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="24"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
-      <c r="F42" s="25"/>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="24"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
-      <c r="F43" s="25"/>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C44" s="16" t="s">
+      <c r="F43" s="24"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C44" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D44" s="17" t="s">
+      <c r="D44" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E44" s="19" t="s">
+      <c r="E44" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F44" s="27"/>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F44" s="26"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B45" s="40" t="s">
+        <v>91</v>
+      </c>
       <c r="C45" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D45" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E45" s="35" t="s">
+      <c r="E45" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="F45" s="29"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F45" s="28"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C46" s="10" t="s">
         <v>22</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E46" s="32" t="s">
+      <c r="E46" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="F46" s="23"/>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F46" s="22"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
-      <c r="F47" s="25"/>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="24"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
-      <c r="F48" s="25"/>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C49" s="16" t="s">
+      <c r="F48" s="24"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C49" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D49" s="17" t="s">
+      <c r="D49" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E49" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E49" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F49" s="21" t="s">
+      <c r="F49" s="20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="8"/>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B50" s="40" t="s">
+        <v>91</v>
+      </c>
       <c r="C50" s="11" t="s">
         <v>34</v>
       </c>
@@ -2256,11 +4443,11 @@
       <c r="E50" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F50" s="24" t="s">
+      <c r="F50" s="23" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C51" s="11" t="s">
         <v>34</v>
       </c>
@@ -2270,11 +4457,11 @@
       <c r="E51" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F51" s="24" t="s">
+      <c r="F51" s="23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="C52" s="11" t="s">
         <v>34</v>
       </c>
@@ -2284,11 +4471,11 @@
       <c r="E52" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F52" s="37" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F52" s="34" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C53" s="11" t="s">
         <v>62</v>
       </c>
@@ -2298,11 +4485,11 @@
       <c r="E53" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F53" s="36" t="s">
+      <c r="F53" s="33" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C54" s="11" t="s">
         <v>28</v>
       </c>
@@ -2312,11 +4499,11 @@
       <c r="E54" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F54" s="24" t="s">
+      <c r="F54" s="23" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C55" s="11" t="s">
         <v>28</v>
       </c>
@@ -2326,11 +4513,11 @@
       <c r="E55" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F55" s="24" t="s">
+      <c r="F55" s="23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C56" s="11" t="s">
         <v>20</v>
       </c>
@@ -2340,50 +4527,53 @@
       <c r="E56" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F56" s="24" t="s">
+      <c r="F56" s="23" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
-      <c r="F57" s="25"/>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F57" s="24"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="3"/>
-      <c r="F58" s="25"/>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B59" s="38" t="s">
-        <v>67</v>
+      <c r="F58" s="24"/>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B59" s="35" t="s">
+        <v>66</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="3"/>
-      <c r="F59" s="25"/>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C60" s="16" t="s">
+      <c r="F59" s="24"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C60" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D60" s="17" t="s">
+      <c r="D60" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E60" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E60" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="F60" s="21" t="s">
+      <c r="F60" s="20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B61" s="40" t="s">
+        <v>91</v>
+      </c>
       <c r="C61" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D61" s="11" t="s">
         <v>16</v>
@@ -2391,13 +4581,16 @@
       <c r="E61" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F61" s="24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F61" s="23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B62" s="40" t="s">
+        <v>91</v>
+      </c>
       <c r="C62" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D62" s="11" t="s">
         <v>43</v>
@@ -2405,13 +4598,16 @@
       <c r="E62" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F62" s="24" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F62" s="23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>92</v>
+      </c>
       <c r="C63" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D63" s="11" t="s">
         <v>29</v>
@@ -2419,13 +4615,16 @@
       <c r="E63" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F63" s="24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F63" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B64" s="40" t="s">
+        <v>91</v>
+      </c>
       <c r="C64" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D64" s="11" t="s">
         <v>29</v>
@@ -2433,41 +4632,41 @@
       <c r="E64" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F64" s="24" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F64" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C65" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D65" s="11" t="s">
         <v>29</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F65" s="24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="F65" s="23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C66" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D66" s="11" t="s">
         <v>29</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F66" s="24" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="F66" s="23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C67" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D67" s="10" t="s">
         <v>43</v>
@@ -2475,13 +4674,13 @@
       <c r="E67" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F67" s="24" t="s">
+      <c r="F67" s="23" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C68" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D68" s="10" t="s">
         <v>29</v>
@@ -2489,13 +4688,13 @@
       <c r="E68" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F68" s="24" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F68" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C69" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D69" s="10" t="s">
         <v>29</v>
@@ -2503,13 +4702,13 @@
       <c r="E69" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F69" s="24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F69" s="23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C70" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D70" s="10" t="s">
         <v>16</v>
@@ -2517,220 +4716,295 @@
       <c r="E70" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F70" s="24" t="s">
+      <c r="F70" s="23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C71" s="39" t="s">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C71" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="D71" s="39" t="s">
+      <c r="D71" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="E71" s="39" t="s">
+      <c r="E71" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F71" s="40" t="s">
+      <c r="F71" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C72" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D72" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E72" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F72" s="37" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C72" s="39" t="s">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C73" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="D72" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="E72" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="F72" s="40" t="s">
+      <c r="D73" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E73" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="F73" s="37" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C73" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="D73" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="E73" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="F73" s="40" t="s">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B74" s="35" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B74" s="38" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C75" s="16" t="s">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C75" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D75" s="17" t="s">
+      <c r="D75" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E75" s="19" t="s">
+      <c r="E75" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F75" s="27"/>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F75" s="26"/>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B76" s="40" t="s">
+        <v>91</v>
+      </c>
       <c r="C76" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D76" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E76" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="F76" s="29"/>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E76" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="F76" s="28"/>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C77" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D77" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E77" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="F77" s="23"/>
+      <c r="E77" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="F77" s="22"/>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E14:F14"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:E5 D32:E33 D28:D31 D6:D23 D35:E43 D46:E48 D45 D57:E59 D61:E65 D67:E74 D78:E1048576">
-    <cfRule type="containsText" dxfId="47" priority="43" operator="containsText" text="Amber">
+    <cfRule type="containsText" dxfId="94" priority="58" operator="containsText" text="Amber">
       <formula>NOT(ISERROR(SEARCH("Amber",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="44" operator="containsText" text="Red">
+    <cfRule type="containsText" dxfId="93" priority="59" operator="containsText" text="Red">
       <formula>NOT(ISERROR(SEARCH("Red",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="45" operator="containsText" text="Green">
+    <cfRule type="containsText" dxfId="92" priority="60" operator="containsText" text="Green">
       <formula>NOT(ISERROR(SEARCH("Green",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24:F27">
-    <cfRule type="containsText" dxfId="44" priority="40" operator="containsText" text="Amber">
+    <cfRule type="containsText" dxfId="91" priority="55" operator="containsText" text="Amber">
       <formula>NOT(ISERROR(SEARCH("Amber",F24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="41" operator="containsText" text="Red">
+    <cfRule type="containsText" dxfId="90" priority="56" operator="containsText" text="Red">
       <formula>NOT(ISERROR(SEARCH("Red",F24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="Green">
+    <cfRule type="containsText" dxfId="89" priority="57" operator="containsText" text="Green">
       <formula>NOT(ISERROR(SEARCH("Green",F24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:D27">
-    <cfRule type="containsText" dxfId="41" priority="37" operator="containsText" text="Amber">
+    <cfRule type="containsText" dxfId="88" priority="52" operator="containsText" text="Amber">
       <formula>NOT(ISERROR(SEARCH("Amber",D24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="38" operator="containsText" text="Red">
+    <cfRule type="containsText" dxfId="87" priority="53" operator="containsText" text="Red">
       <formula>NOT(ISERROR(SEARCH("Red",D24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="Green">
+    <cfRule type="containsText" dxfId="86" priority="54" operator="containsText" text="Green">
       <formula>NOT(ISERROR(SEARCH("Green",D24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44:E44">
-    <cfRule type="containsText" dxfId="38" priority="31" operator="containsText" text="Amber">
+    <cfRule type="containsText" dxfId="85" priority="46" operator="containsText" text="Amber">
       <formula>NOT(ISERROR(SEARCH("Amber",D44)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="32" operator="containsText" text="Red">
+    <cfRule type="containsText" dxfId="84" priority="47" operator="containsText" text="Red">
       <formula>NOT(ISERROR(SEARCH("Red",D44)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="33" operator="containsText" text="Green">
+    <cfRule type="containsText" dxfId="83" priority="48" operator="containsText" text="Green">
       <formula>NOT(ISERROR(SEARCH("Green",D44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D60:E60">
-    <cfRule type="containsText" dxfId="35" priority="10" operator="containsText" text="Amber">
+    <cfRule type="containsText" dxfId="82" priority="25" operator="containsText" text="Amber">
       <formula>NOT(ISERROR(SEARCH("Amber",D60)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="11" operator="containsText" text="Red">
+    <cfRule type="containsText" dxfId="81" priority="26" operator="containsText" text="Red">
       <formula>NOT(ISERROR(SEARCH("Red",D60)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="12" operator="containsText" text="Green">
+    <cfRule type="containsText" dxfId="80" priority="27" operator="containsText" text="Green">
       <formula>NOT(ISERROR(SEARCH("Green",D60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50:E56">
-    <cfRule type="containsText" dxfId="32" priority="25" operator="containsText" text="Amber">
+    <cfRule type="containsText" dxfId="79" priority="40" operator="containsText" text="Amber">
       <formula>NOT(ISERROR(SEARCH("Amber",D50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="26" operator="containsText" text="Red">
+    <cfRule type="containsText" dxfId="78" priority="41" operator="containsText" text="Red">
       <formula>NOT(ISERROR(SEARCH("Red",D50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="27" operator="containsText" text="Green">
+    <cfRule type="containsText" dxfId="77" priority="42" operator="containsText" text="Green">
       <formula>NOT(ISERROR(SEARCH("Green",D50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49:E49">
-    <cfRule type="containsText" dxfId="29" priority="22" operator="containsText" text="Amber">
+    <cfRule type="containsText" dxfId="76" priority="37" operator="containsText" text="Amber">
       <formula>NOT(ISERROR(SEARCH("Amber",D49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="23" operator="containsText" text="Red">
+    <cfRule type="containsText" dxfId="75" priority="38" operator="containsText" text="Red">
       <formula>NOT(ISERROR(SEARCH("Red",D49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="24" operator="containsText" text="Green">
+    <cfRule type="containsText" dxfId="74" priority="39" operator="containsText" text="Green">
       <formula>NOT(ISERROR(SEARCH("Green",D49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34:E34">
-    <cfRule type="containsText" dxfId="26" priority="13" operator="containsText" text="Amber">
+    <cfRule type="containsText" dxfId="73" priority="28" operator="containsText" text="Amber">
       <formula>NOT(ISERROR(SEARCH("Amber",D34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="14" operator="containsText" text="Red">
+    <cfRule type="containsText" dxfId="72" priority="29" operator="containsText" text="Red">
       <formula>NOT(ISERROR(SEARCH("Red",D34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="15" operator="containsText" text="Green">
+    <cfRule type="containsText" dxfId="71" priority="30" operator="containsText" text="Green">
       <formula>NOT(ISERROR(SEARCH("Green",D34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D66:E66">
-    <cfRule type="containsText" dxfId="23" priority="7" operator="containsText" text="Amber">
+    <cfRule type="containsText" dxfId="70" priority="22" operator="containsText" text="Amber">
       <formula>NOT(ISERROR(SEARCH("Amber",D66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="8" operator="containsText" text="Red">
+    <cfRule type="containsText" dxfId="69" priority="23" operator="containsText" text="Red">
       <formula>NOT(ISERROR(SEARCH("Red",D66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="Green">
+    <cfRule type="containsText" dxfId="68" priority="24" operator="containsText" text="Green">
       <formula>NOT(ISERROR(SEARCH("Green",D66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D77:E77 D76">
-    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="Amber">
+    <cfRule type="containsText" dxfId="67" priority="19" operator="containsText" text="Amber">
       <formula>NOT(ISERROR(SEARCH("Amber",D76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="Red">
+    <cfRule type="containsText" dxfId="66" priority="20" operator="containsText" text="Red">
       <formula>NOT(ISERROR(SEARCH("Red",D76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="Green">
+    <cfRule type="containsText" dxfId="65" priority="21" operator="containsText" text="Green">
       <formula>NOT(ISERROR(SEARCH("Green",D76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D75:E75">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Amber">
+    <cfRule type="containsText" dxfId="64" priority="16" operator="containsText" text="Amber">
       <formula>NOT(ISERROR(SEARCH("Amber",D75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Red">
+    <cfRule type="containsText" dxfId="63" priority="17" operator="containsText" text="Red">
       <formula>NOT(ISERROR(SEARCH("Red",D75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Green">
+    <cfRule type="containsText" dxfId="62" priority="18" operator="containsText" text="Green">
       <formula>NOT(ISERROR(SEARCH("Green",D75)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="containsText" dxfId="61" priority="15" operator="containsText" text="*">
+      <formula>NOT(ISERROR(SEARCH("*",B6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22">
+    <cfRule type="containsText" dxfId="60" priority="14" operator="containsText" text="*">
+      <formula>NOT(ISERROR(SEARCH("*",B22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26">
+    <cfRule type="containsText" dxfId="59" priority="13" operator="containsText" text="*">
+      <formula>NOT(ISERROR(SEARCH("*",B26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30">
+    <cfRule type="containsText" dxfId="58" priority="12" operator="containsText" text="*">
+      <formula>NOT(ISERROR(SEARCH("*",B30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="57" priority="11" operator="containsText" text="*">
+      <formula>NOT(ISERROR(SEARCH("*",B30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35">
+    <cfRule type="containsText" dxfId="56" priority="10" operator="containsText" text="*">
+      <formula>NOT(ISERROR(SEARCH("*",B35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45">
+    <cfRule type="containsText" dxfId="55" priority="9" operator="containsText" text="*">
+      <formula>NOT(ISERROR(SEARCH("*",B45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50">
+    <cfRule type="containsText" dxfId="54" priority="8" operator="containsText" text="*">
+      <formula>NOT(ISERROR(SEARCH("*",B50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B61">
+    <cfRule type="containsText" dxfId="53" priority="7" operator="containsText" text="*">
+      <formula>NOT(ISERROR(SEARCH("*",B61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B62">
+    <cfRule type="containsText" dxfId="52" priority="6" operator="containsText" text="*">
+      <formula>NOT(ISERROR(SEARCH("*",B62)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="4" operator="containsText" text="*">
+      <formula>NOT(ISERROR(SEARCH("*",B62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B64">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="*">
+      <formula>NOT(ISERROR(SEARCH("*",B64)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="*">
+      <formula>NOT(ISERROR(SEARCH("*",B64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B76">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="*">
+      <formula>NOT(ISERROR(SEARCH("*",B76)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="*">
+      <formula>NOT(ISERROR(SEARCH("*",B76)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="59" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="59" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -2741,7 +5015,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2753,7 +5027,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>